<commit_message>
Actualización plantilla de ítems de configuración
</commit_message>
<xml_diff>
--- a/Práctico/Trabajos Prácticos/Evaluables/TP N° 4/Documento_Salida_Plantilla_de_Ítems_de_Configuración.xlsx
+++ b/Práctico/Trabajos Prácticos/Evaluables/TP N° 4/Documento_Salida_Plantilla_de_Ítems_de_Configuración.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Joaquin2\Estudio\Ingenieria en Sistemas\4to Año\ISW - Ingeniería de Software\TP Evaluables\TP N° 4-5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7F1CD7-E52E-4800-AAB0-93A6DB904363}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881A84D0-9A3A-4C98-B8D8-EA8BD4239DA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -172,9 +172,6 @@
     <t>Modalidad_Académica_ISW_2019.pdf</t>
   </si>
   <si>
-    <t>US_&lt;Nro&gt;_&lt;NombreUS&gt;.docx</t>
-  </si>
-  <si>
     <t>&lt;NombreArchivo&gt;.&lt;extension&gt;</t>
   </si>
   <si>
@@ -314,9 +311,6 @@
     <t>Documento de salida de TP Evaluable</t>
   </si>
   <si>
-    <t>Los ítems de configuración "Libro", "Foto Registro de Trabajo Práctico Resuelto", "Enunciado Trabajo Práctico Adicional", "Material de Entrada", "Foto Registro de TP Evaluable", "User Storie de TP Evaluable", "Documento de entrada de TP Evaluable" y "Documento de salida de TP Evaluable" son opcionales de acuerdo a las características del enunciado</t>
-  </si>
-  <si>
     <t>&lt;NombreLibro&gt; - &lt;AutorLibro&gt; - &lt;EdiciónLibro&gt;.&lt;extension&gt;</t>
   </si>
   <si>
@@ -326,12 +320,6 @@
     <t>&lt;EdiciónLibro&gt;: Edición particular del libro</t>
   </si>
   <si>
-    <t>&lt;NombreDominio&gt;: Indica de que dominio se trata dentro del TP N° N</t>
-  </si>
-  <si>
-    <t>&lt;NombreDominio&gt;_Foto_N°_&lt;Nro&gt;_&lt;Autor&gt;.jpg</t>
-  </si>
-  <si>
     <t>&lt;Autor&gt;: Indica integrante de grupo a quien corresponde el archivo</t>
   </si>
   <si>
@@ -354,6 +342,18 @@
   </si>
   <si>
     <t>ISW_Grupo2_2019/</t>
+  </si>
+  <si>
+    <t>US_&lt;NombreUS&gt;.docx</t>
+  </si>
+  <si>
+    <t>&lt;N° Caso Práctico&gt;_Foto_N°_&lt;Nro&gt;_&lt;Autor&gt;.jpg</t>
+  </si>
+  <si>
+    <t>&lt;N° Caso Práctico&gt;: Indica de que caso práctico se trata dentro del TP N° N</t>
+  </si>
+  <si>
+    <t>Los ítems de configuración "Libro", "Foto Registro de Trabajo Práctico Resuelto", "Enunciado Trabajo Práctico Adicional", "Foto Registro de Trabajo Práctico Adicional", "Material de Entrada", "Foto Registro de TP Evaluable", "User Storie de TP Evaluable", "Documento de entrada de TP Evaluable" y "Documento de salida de TP Evaluable" son opcionales de acuerdo a las características del enunciado</t>
   </si>
 </sst>
 </file>
@@ -788,10 +788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:U39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,7 +800,7 @@
     <col min="2" max="2" width="56" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="108" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="45.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
     <col min="9" max="9" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -823,10 +823,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>47</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>12</v>
@@ -879,7 +879,7 @@
         <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>16</v>
@@ -890,13 +890,13 @@
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>33</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>34</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>12</v>
@@ -904,13 +904,13 @@
     </row>
     <row r="8" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>13</v>
@@ -923,13 +923,13 @@
     </row>
     <row r="9" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>12</v>
@@ -942,13 +942,13 @@
     </row>
     <row r="10" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>13</v>
@@ -961,13 +961,13 @@
     </row>
     <row r="11" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>44</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>12</v>
@@ -980,13 +980,13 @@
     </row>
     <row r="12" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>13</v>
@@ -999,13 +999,13 @@
     </row>
     <row r="13" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>13</v>
@@ -1018,13 +1018,13 @@
     </row>
     <row r="14" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>12</v>
@@ -1037,13 +1037,13 @@
     </row>
     <row r="15" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>12</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="16" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>13</v>
@@ -1077,7 +1077,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>20</v>
@@ -1131,13 +1131,13 @@
     </row>
     <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>12</v>
@@ -1170,62 +1170,62 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
@@ -1234,8 +1234,21 @@
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
       <c r="H38" s="10"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
+      <c r="N38" s="10"/>
+      <c r="O38" s="10"/>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="10"/>
+      <c r="R38" s="10"/>
+      <c r="S38" s="10"/>
+      <c r="T38" s="10"/>
+      <c r="U38" s="10"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
@@ -1243,7 +1256,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A38:H38"/>
+    <mergeCell ref="A38:U38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Cambio de nombres de archivos segun plantilla de items de configuración
</commit_message>
<xml_diff>
--- a/Práctico/Trabajos Prácticos/Evaluables/TP N° 4/Documento_Salida_Plantilla_de_Ítems_de_Configuración.xlsx
+++ b/Práctico/Trabajos Prácticos/Evaluables/TP N° 4/Documento_Salida_Plantilla_de_Ítems_de_Configuración.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Joaquin2\Estudio\Ingenieria en Sistemas\4to Año\ISW - Ingeniería de Software\TP Evaluables\TP N° 4-5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce3\Documents\GitHub\ISW_Grupo2_2019\Práctico\Trabajos Prácticos\Evaluables\TP N° 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881A84D0-9A3A-4C98-B8D8-EA8BD4239DA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841CC8DF-C9D0-4AEF-BACC-587B26F3CDAB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="17310" windowHeight="9810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -311,9 +311,6 @@
     <t>Documento de salida de TP Evaluable</t>
   </si>
   <si>
-    <t>&lt;NombreLibro&gt; - &lt;AutorLibro&gt; - &lt;EdiciónLibro&gt;.&lt;extension&gt;</t>
-  </si>
-  <si>
     <t>&lt;AutorLibro&gt;: Autor/es del libro</t>
   </si>
   <si>
@@ -354,6 +351,9 @@
   </si>
   <si>
     <t>Los ítems de configuración "Libro", "Foto Registro de Trabajo Práctico Resuelto", "Enunciado Trabajo Práctico Adicional", "Foto Registro de Trabajo Práctico Adicional", "Material de Entrada", "Foto Registro de TP Evaluable", "User Storie de TP Evaluable", "Documento de entrada de TP Evaluable" y "Documento de salida de TP Evaluable" son opcionales de acuerdo a las características del enunciado</t>
+  </si>
+  <si>
+    <t>&lt;NombreLibro&gt;_&lt;AutorLibro&gt;_&lt;EdiciónLibro&gt;.&lt;extension&gt;</t>
   </si>
 </sst>
 </file>
@@ -468,11 +468,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -492,7 +492,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -791,10 +791,10 @@
   <dimension ref="A1:U39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43" customWidth="1"/>
     <col min="2" max="2" width="56" bestFit="1" customWidth="1"/>
@@ -879,7 +879,7 @@
         <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>16</v>
@@ -907,7 +907,7 @@
         <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>34</v>
@@ -980,10 +980,10 @@
     </row>
     <row r="12" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>38</v>
@@ -992,7 +992,7 @@
         <v>13</v>
       </c>
       <c r="G12" s="3"/>
-      <c r="H12" s="12"/>
+      <c r="H12" s="11"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -1021,7 +1021,7 @@
         <v>39</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>38</v>
@@ -1040,7 +1040,7 @@
         <v>44</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>38</v>
@@ -1059,7 +1059,7 @@
         <v>57</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>38</v>
@@ -1131,13 +1131,13 @@
     </row>
     <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>12</v>
@@ -1190,7 +1190,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -1200,12 +1200,12 @@
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
@@ -1220,39 +1220,39 @@
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
-      <c r="K38" s="10"/>
-      <c r="L38" s="10"/>
-      <c r="M38" s="10"/>
-      <c r="N38" s="10"/>
-      <c r="O38" s="10"/>
-      <c r="P38" s="10"/>
-      <c r="Q38" s="10"/>
-      <c r="R38" s="10"/>
-      <c r="S38" s="10"/>
-      <c r="T38" s="10"/>
-      <c r="U38" s="10"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="12"/>
+      <c r="N38" s="12"/>
+      <c r="O38" s="12"/>
+      <c r="P38" s="12"/>
+      <c r="Q38" s="12"/>
+      <c r="R38" s="12"/>
+      <c r="S38" s="12"/>
+      <c r="T38" s="12"/>
+      <c r="U38" s="12"/>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A39" s="11"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Actualización plantilla de items de configuración
</commit_message>
<xml_diff>
--- a/Práctico/Trabajos Prácticos/Evaluables/TP N° 4/Documento_Salida_Plantilla_de_Ítems_de_Configuración.xlsx
+++ b/Práctico/Trabajos Prácticos/Evaluables/TP N° 4/Documento_Salida_Plantilla_de_Ítems_de_Configuración.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce3\Documents\GitHub\ISW_Grupo2_2019\Práctico\Trabajos Prácticos\Evaluables\TP N° 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Joaquin2\Estudio\Ingenieria en Sistemas\4to Año\ISW - Ingeniería de Software\TP Evaluables\TP N° 4-5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841CC8DF-C9D0-4AEF-BACC-587B26F3CDAB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA04487-0F76-4717-B9E5-060A88EF03CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="17310" windowHeight="9810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -261,9 +261,6 @@
     <t>Documento de entrada de TP Evaluable</t>
   </si>
   <si>
-    <t>&lt;NombreTema&gt;.pdf</t>
-  </si>
-  <si>
     <r>
       <t>ISW_Grupo2_2019</t>
     </r>
@@ -311,6 +308,9 @@
     <t>Documento de salida de TP Evaluable</t>
   </si>
   <si>
+    <t>&lt;NombreLibro&gt; - &lt;AutorLibro&gt; - &lt;EdiciónLibro&gt;.&lt;extension&gt;</t>
+  </si>
+  <si>
     <t>&lt;AutorLibro&gt;: Autor/es del libro</t>
   </si>
   <si>
@@ -353,7 +353,7 @@
     <t>Los ítems de configuración "Libro", "Foto Registro de Trabajo Práctico Resuelto", "Enunciado Trabajo Práctico Adicional", "Foto Registro de Trabajo Práctico Adicional", "Material de Entrada", "Foto Registro de TP Evaluable", "User Storie de TP Evaluable", "Documento de entrada de TP Evaluable" y "Documento de salida de TP Evaluable" son opcionales de acuerdo a las características del enunciado</t>
   </si>
   <si>
-    <t>&lt;NombreLibro&gt;_&lt;AutorLibro&gt;_&lt;EdiciónLibro&gt;.&lt;extension&gt;</t>
+    <t>&lt;Nro&gt;_&lt;NombreTema&gt;.pdf</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -791,10 +791,10 @@
   <dimension ref="A1:U39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43" customWidth="1"/>
     <col min="2" max="2" width="56" bestFit="1" customWidth="1"/>
@@ -823,10 +823,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>45</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>46</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>12</v>
@@ -879,7 +879,7 @@
         <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>16</v>
@@ -923,10 +923,10 @@
     </row>
     <row r="9" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>36</v>
@@ -942,10 +942,10 @@
     </row>
     <row r="10" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>36</v>
@@ -1056,7 +1056,7 @@
     </row>
     <row r="16" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>63</v>
@@ -1175,17 +1175,17 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -1195,7 +1195,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
@@ -1210,12 +1210,12 @@
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>